<commit_message>
double checking standardization of description , typo catches
</commit_message>
<xml_diff>
--- a/data/expt_2/raw_transcripts/game25.xlsx
+++ b/data/expt_2/raw_transcripts/game25.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="179">
   <si>
     <t xml:space="preserve">start</t>
   </si>
@@ -434,9 +434,6 @@
   </si>
   <si>
     <t xml:space="preserve">Boat.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">boat</t>
   </si>
   <si>
     <t xml:space="preserve">Awesome!</t>
@@ -655,20 +652,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -864,2770 +865,2766 @@
   <dimension ref="A1:I168"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A138" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F166" activeCellId="0" sqref="F166"/>
+      <selection pane="bottomLeft" activeCell="H123" activeCellId="0" sqref="H123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="37.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="37.65"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" s="2" t="n">
         <v>2000</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+      <c r="A3" s="2" t="n">
         <v>2000</v>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="B3" s="2" t="n">
         <v>11500</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+      <c r="A4" s="2" t="n">
         <v>11500</v>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="B4" s="2" t="n">
         <v>13500</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
+      <c r="A5" s="2" t="n">
         <v>13500</v>
       </c>
-      <c r="B5" s="1" t="n">
+      <c r="B5" s="2" t="n">
         <v>14000</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
+      <c r="A6" s="2" t="n">
         <v>14000</v>
       </c>
-      <c r="B6" s="1" t="n">
+      <c r="B6" s="2" t="n">
         <v>16500</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
+      <c r="A7" s="2" t="n">
         <v>16500</v>
       </c>
-      <c r="B7" s="1" t="n">
+      <c r="B7" s="2" t="n">
         <v>20000</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
+      <c r="A8" s="2" t="n">
         <v>20000</v>
       </c>
-      <c r="B8" s="1" t="n">
+      <c r="B8" s="2" t="n">
         <v>22000</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
+      <c r="A9" s="2" t="n">
         <v>22000</v>
       </c>
-      <c r="B9" s="1" t="n">
+      <c r="B9" s="2" t="n">
         <v>26000</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
+      <c r="A10" s="2" t="n">
         <v>26000</v>
       </c>
-      <c r="B10" s="1" t="n">
+      <c r="B10" s="2" t="n">
         <v>29000</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
+      <c r="A11" s="2" t="n">
         <v>29000</v>
       </c>
-      <c r="B11" s="1" t="n">
+      <c r="B11" s="2" t="n">
         <v>31000</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="n">
+      <c r="A12" s="2" t="n">
         <v>31000</v>
       </c>
-      <c r="B12" s="1" t="n">
+      <c r="B12" s="2" t="n">
         <v>35000</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
+      <c r="A13" s="2" t="n">
         <v>35000</v>
       </c>
-      <c r="B13" s="1" t="n">
+      <c r="B13" s="2" t="n">
         <v>36000</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
+      <c r="A14" s="2" t="n">
         <v>36000</v>
       </c>
-      <c r="B14" s="1" t="n">
+      <c r="B14" s="2" t="n">
         <v>37000</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="n">
+      <c r="A15" s="2" t="n">
         <v>37000</v>
       </c>
-      <c r="B15" s="1" t="n">
+      <c r="B15" s="2" t="n">
         <v>38000</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="n">
+      <c r="A16" s="2" t="n">
         <v>38000</v>
       </c>
-      <c r="B16" s="1" t="n">
+      <c r="B16" s="2" t="n">
         <v>39000</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="n">
+      <c r="A17" s="2" t="n">
         <v>39000</v>
       </c>
-      <c r="B17" s="1" t="n">
+      <c r="B17" s="2" t="n">
         <v>42000</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="n">
+      <c r="A18" s="2" t="n">
         <v>42000</v>
       </c>
-      <c r="B18" s="1" t="n">
+      <c r="B18" s="2" t="n">
         <v>43000</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="n">
+      <c r="A19" s="2" t="n">
         <v>42000</v>
       </c>
-      <c r="B19" s="1" t="n">
+      <c r="B19" s="2" t="n">
         <v>43000</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="n">
+      <c r="A20" s="2" t="n">
         <v>43000</v>
       </c>
-      <c r="B20" s="1" t="n">
+      <c r="B20" s="2" t="n">
         <v>46000</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="n">
+      <c r="A21" s="2" t="n">
         <v>46000</v>
       </c>
-      <c r="B21" s="1" t="n">
+      <c r="B21" s="2" t="n">
         <v>49000</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="n">
+      <c r="A22" s="2" t="n">
         <v>49000</v>
       </c>
-      <c r="B22" s="1" t="n">
+      <c r="B22" s="2" t="n">
         <v>50000</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="n">
+      <c r="A23" s="2" t="n">
         <v>50000</v>
       </c>
-      <c r="B23" s="1" t="n">
+      <c r="B23" s="2" t="n">
         <v>51000</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="n">
+      <c r="A24" s="2" t="n">
         <v>51000</v>
       </c>
-      <c r="B24" s="1" t="n">
+      <c r="B24" s="2" t="n">
         <v>52000</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="n">
+      <c r="A25" s="2" t="n">
         <v>52000</v>
       </c>
-      <c r="B25" s="1" t="n">
+      <c r="B25" s="2" t="n">
         <v>53000</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="n">
+      <c r="A26" s="2" t="n">
         <v>52000</v>
       </c>
-      <c r="B26" s="1" t="n">
+      <c r="B26" s="2" t="n">
         <v>53000</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="n">
+      <c r="A27" s="2" t="n">
         <v>53000</v>
       </c>
-      <c r="B27" s="1" t="n">
+      <c r="B27" s="2" t="n">
         <v>58360</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="n">
+      <c r="A28" s="2" t="n">
         <v>59560</v>
       </c>
-      <c r="B28" s="1" t="n">
+      <c r="B28" s="2" t="n">
         <v>64080</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="n">
+      <c r="A29" s="2" t="n">
         <v>64200</v>
       </c>
-      <c r="B29" s="1" t="n">
+      <c r="B29" s="2" t="n">
         <v>64940</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="n">
+      <c r="A30" s="2" t="n">
         <v>64200</v>
       </c>
-      <c r="B30" s="1" t="n">
+      <c r="B30" s="2" t="n">
         <v>64940</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D30" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="n">
+      <c r="A31" s="2" t="n">
         <v>65580</v>
       </c>
-      <c r="B31" s="1" t="n">
+      <c r="B31" s="2" t="n">
         <v>72460</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="n">
+      <c r="A32" s="2" t="n">
         <v>73560</v>
       </c>
-      <c r="B32" s="1" t="n">
+      <c r="B32" s="2" t="n">
         <v>77740</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="n">
+      <c r="A33" s="2" t="n">
         <v>77740</v>
       </c>
-      <c r="B33" s="1" t="n">
+      <c r="B33" s="2" t="n">
         <v>84480</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D33" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="n">
+      <c r="A34" s="2" t="n">
         <v>85600</v>
       </c>
-      <c r="B34" s="1" t="n">
+      <c r="B34" s="2" t="n">
         <v>88740</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D34" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="n">
+      <c r="A35" s="2" t="n">
         <v>88740</v>
       </c>
-      <c r="B35" s="1" t="n">
+      <c r="B35" s="2" t="n">
         <v>93740</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D35" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="n">
+      <c r="A36" s="2" t="n">
         <v>93740</v>
       </c>
-      <c r="B36" s="1" t="n">
+      <c r="B36" s="2" t="n">
         <v>96740</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D36" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="n">
+      <c r="A37" s="2" t="n">
         <v>96740</v>
       </c>
-      <c r="B37" s="1" t="n">
+      <c r="B37" s="2" t="n">
         <v>98740</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D37" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="n">
+      <c r="A38" s="2" t="n">
         <v>98740</v>
       </c>
-      <c r="B38" s="1" t="n">
+      <c r="B38" s="2" t="n">
         <v>99740</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D38" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="n">
+      <c r="A39" s="2" t="n">
         <v>99740</v>
       </c>
-      <c r="B39" s="1" t="n">
+      <c r="B39" s="2" t="n">
         <v>100740</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D39" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="n">
+      <c r="A40" s="2" t="n">
         <v>100740</v>
       </c>
-      <c r="B40" s="1" t="n">
+      <c r="B40" s="2" t="n">
         <v>101740</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D40" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="n">
+      <c r="A41" s="2" t="n">
         <v>101740</v>
       </c>
-      <c r="B41" s="1" t="n">
+      <c r="B41" s="2" t="n">
         <v>104740</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D41" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="n">
+      <c r="A42" s="2" t="n">
         <v>104740</v>
       </c>
-      <c r="B42" s="1" t="n">
+      <c r="B42" s="2" t="n">
         <v>106740</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D42" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="n">
+      <c r="A43" s="2" t="n">
         <v>106740</v>
       </c>
-      <c r="B43" s="1" t="n">
+      <c r="B43" s="2" t="n">
         <v>108740</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D43" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="n">
+      <c r="A44" s="2" t="n">
         <v>108740</v>
       </c>
-      <c r="B44" s="1" t="n">
+      <c r="B44" s="2" t="n">
         <v>109740</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C44" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D44" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="n">
+      <c r="A45" s="2" t="n">
         <v>109740</v>
       </c>
-      <c r="B45" s="1" t="n">
+      <c r="B45" s="2" t="n">
         <v>112160</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C45" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D45" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="n">
+      <c r="A46" s="2" t="n">
         <v>112260</v>
       </c>
-      <c r="B46" s="1" t="n">
+      <c r="B46" s="2" t="n">
         <v>114280</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C46" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D46" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="n">
+      <c r="A47" s="2" t="n">
         <v>114280</v>
       </c>
-      <c r="B47" s="1" t="n">
+      <c r="B47" s="2" t="n">
         <v>116280</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C47" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D47" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="n">
+      <c r="A48" s="2" t="n">
         <v>116860</v>
       </c>
-      <c r="B48" s="1" t="n">
+      <c r="B48" s="2" t="n">
         <v>117520</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D48" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="n">
+      <c r="A49" s="2" t="n">
         <v>117680</v>
       </c>
-      <c r="B49" s="1" t="n">
+      <c r="B49" s="2" t="n">
         <v>117800</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C49" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="D49" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="n">
+      <c r="A50" s="2" t="n">
         <v>117920</v>
       </c>
-      <c r="B50" s="1" t="n">
+      <c r="B50" s="2" t="n">
         <v>118580</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C50" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D50" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="n">
+      <c r="A51" s="2" t="n">
         <v>118980</v>
       </c>
-      <c r="B51" s="1" t="n">
+      <c r="B51" s="2" t="n">
         <v>119220</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C51" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D51" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="n">
+      <c r="A52" s="2" t="n">
         <v>119400</v>
       </c>
-      <c r="B52" s="1" t="n">
+      <c r="B52" s="2" t="n">
         <v>119720</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C52" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="D52" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1" t="n">
+      <c r="A53" s="2" t="n">
         <v>120980</v>
       </c>
-      <c r="B53" s="1" t="n">
+      <c r="B53" s="2" t="n">
         <v>123680</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C53" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D53" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="1" t="n">
+      <c r="A54" s="2" t="n">
         <v>124440</v>
       </c>
-      <c r="B54" s="1" t="n">
+      <c r="B54" s="2" t="n">
         <v>125080</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C54" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="D54" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="1" t="n">
+      <c r="A55" s="2" t="n">
         <v>125660</v>
       </c>
-      <c r="B55" s="1" t="n">
+      <c r="B55" s="2" t="n">
         <v>126180</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C55" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="D55" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="1" t="n">
+      <c r="A56" s="2" t="n">
         <v>126620</v>
       </c>
-      <c r="B56" s="1" t="n">
+      <c r="B56" s="2" t="n">
         <v>127020</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C56" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D56" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="1" t="n">
+      <c r="A57" s="2" t="n">
         <v>127420</v>
       </c>
-      <c r="B57" s="1" t="n">
+      <c r="B57" s="2" t="n">
         <v>128660</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C57" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D57" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E57" s="1" t="n">
+      <c r="D57" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E57" s="2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="n">
+      <c r="A58" s="2" t="n">
         <v>128760</v>
       </c>
-      <c r="B58" s="1" t="n">
+      <c r="B58" s="2" t="n">
         <v>128960</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C58" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="D58" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F58" s="1" t="s">
+      <c r="F58" s="2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="1" t="n">
+      <c r="A59" s="2" t="n">
         <v>129500</v>
       </c>
-      <c r="B59" s="1" t="n">
+      <c r="B59" s="2" t="n">
         <v>129780</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C59" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="D59" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="1" t="n">
+      <c r="A60" s="2" t="n">
         <v>129780</v>
       </c>
-      <c r="B60" s="1" t="n">
+      <c r="B60" s="2" t="n">
         <v>134560</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C60" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="D60" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="1" t="n">
+      <c r="A61" s="2" t="n">
         <v>129780</v>
       </c>
-      <c r="B61" s="1" t="n">
+      <c r="B61" s="2" t="n">
         <v>134560</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C61" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D61" s="1" t="s">
+      <c r="D61" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F61" s="1" t="s">
+      <c r="F61" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="H61" s="1" t="s">
+      <c r="H61" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="I61" s="2" t="s">
+      <c r="I61" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="1" t="n">
+      <c r="A62" s="2" t="n">
         <v>135280</v>
       </c>
-      <c r="B62" s="1" t="n">
+      <c r="B62" s="2" t="n">
         <v>141720</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C62" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D62" s="1" t="s">
+      <c r="D62" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="1" t="n">
+      <c r="A63" s="2" t="n">
         <v>135280</v>
       </c>
-      <c r="B63" s="1" t="n">
+      <c r="B63" s="2" t="n">
         <v>141720</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C63" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D63" s="1" t="s">
+      <c r="D63" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F63" s="1" t="s">
+      <c r="F63" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="H63" s="1" t="s">
+      <c r="H63" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="I63" s="2" t="s">
+      <c r="I63" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="1" t="n">
+      <c r="A64" s="2" t="n">
         <v>142160</v>
       </c>
-      <c r="B64" s="1" t="n">
+      <c r="B64" s="2" t="n">
         <v>150440</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C64" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D64" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E64" s="1" t="n">
+      <c r="D64" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E64" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="1" t="n">
+      <c r="A65" s="2" t="n">
         <v>150600</v>
       </c>
-      <c r="B65" s="1" t="n">
+      <c r="B65" s="2" t="n">
         <v>158380</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C65" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="D65" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="1" t="n">
+      <c r="A66" s="2" t="n">
         <v>158380</v>
       </c>
-      <c r="B66" s="1" t="n">
+      <c r="B66" s="2" t="n">
         <v>160620</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C66" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D66" s="1" t="s">
+      <c r="D66" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F66" s="1" t="s">
+      <c r="F66" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="H66" s="1" t="s">
+      <c r="H66" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="I66" s="2" t="s">
+      <c r="I66" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="1" t="n">
+      <c r="A67" s="2" t="n">
         <v>160620</v>
       </c>
-      <c r="B67" s="1" t="n">
+      <c r="B67" s="2" t="n">
         <v>163980</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C67" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D67" s="1" t="s">
+      <c r="D67" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="1" t="n">
+      <c r="A68" s="2" t="n">
         <v>169020</v>
       </c>
-      <c r="B68" s="1" t="n">
+      <c r="B68" s="2" t="n">
         <v>170220</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C68" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D68" s="1" t="s">
+      <c r="D68" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F68" s="1" t="s">
+      <c r="F68" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="H68" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="I68" s="2" t="s">
+      <c r="H68" s="2"/>
+      <c r="I68" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="1" t="n">
+      <c r="A69" s="2" t="n">
         <v>170860</v>
       </c>
-      <c r="B69" s="1" t="n">
+      <c r="B69" s="2" t="n">
         <v>171980</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="C69" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D69" s="1" t="s">
+      <c r="D69" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="1" t="n">
+      <c r="A70" s="2" t="n">
         <v>172620</v>
       </c>
-      <c r="B70" s="1" t="n">
+      <c r="B70" s="2" t="n">
         <v>173660</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C70" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D70" s="1" t="s">
+      <c r="D70" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F70" s="1" t="s">
+      <c r="F70" s="2" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="1" t="n">
+      <c r="A71" s="2" t="n">
         <v>174620</v>
       </c>
-      <c r="B71" s="1" t="n">
+      <c r="B71" s="2" t="n">
         <v>177420</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="C71" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D71" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E71" s="1" t="n">
+      <c r="D71" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E71" s="2" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="1" t="n">
+      <c r="A72" s="2" t="n">
         <v>177420</v>
       </c>
-      <c r="B72" s="1" t="n">
+      <c r="B72" s="2" t="n">
         <v>178300</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C72" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D72" s="1" t="s">
+      <c r="D72" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F72" s="1" t="s">
+      <c r="F72" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="H72" s="1" t="s">
+      <c r="H72" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="I72" s="2" t="s">
+      <c r="I72" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="1" t="n">
+      <c r="A73" s="2" t="n">
         <v>177420</v>
       </c>
-      <c r="B73" s="1" t="n">
+      <c r="B73" s="2" t="n">
         <v>178300</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="C73" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D73" s="1" t="s">
+      <c r="D73" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F73" s="1" t="s">
+      <c r="F73" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="H73" s="1" t="s">
+      <c r="H73" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I73" s="2" t="s">
+      <c r="I73" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="1" t="n">
+      <c r="A74" s="2" t="n">
         <v>180220</v>
       </c>
-      <c r="B74" s="1" t="n">
+      <c r="B74" s="2" t="n">
         <v>181900</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="C74" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D74" s="1" t="s">
+      <c r="D74" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F74" s="1" t="s">
+      <c r="F74" s="2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="1" t="n">
+      <c r="A75" s="2" t="n">
         <v>183660</v>
       </c>
-      <c r="B75" s="1" t="n">
+      <c r="B75" s="2" t="n">
         <v>186700</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="C75" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D75" s="1" t="s">
+      <c r="D75" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="1" t="n">
+      <c r="A76" s="2" t="n">
         <v>186700</v>
       </c>
-      <c r="B76" s="1" t="n">
+      <c r="B76" s="2" t="n">
         <v>190300</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="C76" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D76" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E76" s="1" t="n">
+      <c r="D76" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E76" s="2" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="1" t="n">
+      <c r="A77" s="2" t="n">
         <v>190300</v>
       </c>
-      <c r="B77" s="1" t="n">
+      <c r="B77" s="2" t="n">
         <v>192020</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="C77" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D77" s="1" t="s">
+      <c r="D77" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F77" s="1" t="s">
+      <c r="F77" s="2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="1" t="n">
+      <c r="A78" s="2" t="n">
         <v>192020</v>
       </c>
-      <c r="B78" s="1" t="n">
+      <c r="B78" s="2" t="n">
         <v>193020</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C78" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D78" s="1" t="s">
+      <c r="D78" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="1" t="n">
+      <c r="A79" s="2" t="n">
         <v>193020</v>
       </c>
-      <c r="B79" s="1" t="n">
+      <c r="B79" s="2" t="n">
         <v>194020</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="C79" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D79" s="1" t="s">
+      <c r="D79" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F79" s="1" t="s">
+      <c r="F79" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="H79" s="1" t="s">
+      <c r="H79" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="I79" s="2" t="s">
+      <c r="I79" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="1" t="n">
+      <c r="A80" s="2" t="n">
         <v>194020</v>
       </c>
-      <c r="B80" s="1" t="n">
+      <c r="B80" s="2" t="n">
         <v>196020</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="C80" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D80" s="1" t="s">
+      <c r="D80" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="1" t="n">
+      <c r="A81" s="2" t="n">
         <v>196020</v>
       </c>
-      <c r="B81" s="1" t="n">
+      <c r="B81" s="2" t="n">
         <v>197020</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="C81" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D81" s="1" t="s">
+      <c r="D81" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="1" t="n">
+      <c r="A82" s="2" t="n">
         <v>197020</v>
       </c>
-      <c r="B82" s="1" t="n">
+      <c r="B82" s="2" t="n">
         <v>199220</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="C82" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D82" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E82" s="1" t="n">
+      <c r="D82" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E82" s="2" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="1" t="n">
+      <c r="A83" s="2" t="n">
         <v>199220</v>
       </c>
-      <c r="B83" s="1" t="n">
+      <c r="B83" s="2" t="n">
         <v>203820</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="C83" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D83" s="1" t="s">
+      <c r="D83" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="1" t="n">
+      <c r="A84" s="2" t="n">
         <v>203820</v>
       </c>
-      <c r="B84" s="1" t="n">
+      <c r="B84" s="2" t="n">
         <v>206360</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="C84" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D84" s="1" t="s">
+      <c r="D84" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F84" s="1" t="s">
+      <c r="F84" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I84" s="2" t="s">
+      <c r="I84" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="1" t="n">
+      <c r="A85" s="2" t="n">
         <v>206360</v>
       </c>
-      <c r="B85" s="1" t="n">
+      <c r="B85" s="2" t="n">
         <v>208620</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="C85" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D85" s="1" t="s">
+      <c r="D85" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="1" t="n">
+      <c r="A86" s="2" t="n">
         <v>208620</v>
       </c>
-      <c r="B86" s="1" t="n">
+      <c r="B86" s="2" t="n">
         <v>209620</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="C86" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D86" s="1" t="s">
+      <c r="D86" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F86" s="1" t="s">
+      <c r="F86" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I86" s="2" t="s">
+      <c r="I86" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="1" t="n">
+      <c r="A87" s="2" t="n">
         <v>209620</v>
       </c>
-      <c r="B87" s="1" t="n">
+      <c r="B87" s="2" t="n">
         <v>210620</v>
       </c>
-      <c r="C87" s="1" t="s">
+      <c r="C87" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D87" s="1" t="s">
+      <c r="D87" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="1" t="n">
+      <c r="A88" s="2" t="n">
         <v>210620</v>
       </c>
-      <c r="B88" s="1" t="n">
+      <c r="B88" s="2" t="n">
         <v>211620</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="C88" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D88" s="1" t="s">
+      <c r="D88" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="1" t="n">
+      <c r="A89" s="2" t="n">
         <v>211620</v>
       </c>
-      <c r="B89" s="1" t="n">
+      <c r="B89" s="2" t="n">
         <v>212620</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="C89" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D89" s="1" t="s">
+      <c r="D89" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="1" t="n">
+      <c r="A90" s="2" t="n">
         <v>212620</v>
       </c>
-      <c r="B90" s="1" t="n">
+      <c r="B90" s="2" t="n">
         <v>216620</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="C90" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D90" s="1" t="s">
+      <c r="D90" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F90" s="1" t="s">
+      <c r="F90" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I90" s="2" t="s">
+      <c r="I90" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="1" t="n">
+      <c r="A91" s="2" t="n">
         <v>216620</v>
       </c>
-      <c r="B91" s="1" t="n">
+      <c r="B91" s="2" t="n">
         <v>217620</v>
       </c>
-      <c r="C91" s="1" t="s">
+      <c r="C91" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D91" s="1" t="s">
+      <c r="D91" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F91" s="1" t="s">
+      <c r="F91" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="H91" s="1" t="s">
+      <c r="H91" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="I91" s="2" t="s">
+      <c r="I91" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="1" t="n">
+      <c r="A92" s="2" t="n">
         <v>217620</v>
       </c>
-      <c r="B92" s="1" t="n">
+      <c r="B92" s="2" t="n">
         <v>222620</v>
       </c>
-      <c r="C92" s="1" t="s">
+      <c r="C92" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D92" s="1" t="s">
+      <c r="D92" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="1" t="n">
+      <c r="A93" s="2" t="n">
         <v>222620</v>
       </c>
-      <c r="B93" s="1" t="n">
+      <c r="B93" s="2" t="n">
         <v>224620</v>
       </c>
-      <c r="C93" s="1" t="s">
+      <c r="C93" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D93" s="1" t="s">
+      <c r="D93" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F93" s="1" t="s">
+      <c r="F93" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="H93" s="1" t="s">
+      <c r="H93" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="I93" s="2" t="s">
+      <c r="I93" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="1" t="n">
+      <c r="A94" s="2" t="n">
         <v>224620</v>
       </c>
-      <c r="B94" s="1" t="n">
+      <c r="B94" s="2" t="n">
         <v>226620</v>
       </c>
-      <c r="C94" s="1" t="s">
+      <c r="C94" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D94" s="1" t="s">
+      <c r="D94" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F94" s="1" t="s">
+      <c r="F94" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="H94" s="1" t="s">
+      <c r="H94" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="I94" s="2" t="s">
+      <c r="I94" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="1" t="n">
+      <c r="A95" s="2" t="n">
         <v>226620</v>
       </c>
-      <c r="B95" s="1" t="n">
+      <c r="B95" s="2" t="n">
         <v>227620</v>
       </c>
-      <c r="C95" s="1" t="s">
+      <c r="C95" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D95" s="1" t="s">
+      <c r="D95" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F95" s="1" t="s">
+      <c r="F95" s="2" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="1" t="n">
+      <c r="A96" s="2" t="n">
         <v>226620</v>
       </c>
-      <c r="B96" s="1" t="n">
+      <c r="B96" s="2" t="n">
         <v>227620</v>
       </c>
-      <c r="C96" s="1" t="s">
+      <c r="C96" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D96" s="1" t="s">
+      <c r="D96" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F96" s="1" t="s">
+      <c r="F96" s="2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="1" t="n">
+      <c r="A97" s="2" t="n">
         <v>227620</v>
       </c>
-      <c r="B97" s="1" t="n">
+      <c r="B97" s="2" t="n">
         <v>228620</v>
       </c>
-      <c r="C97" s="1" t="s">
+      <c r="C97" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D97" s="1" t="s">
+      <c r="D97" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F97" s="1" t="s">
+      <c r="F97" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="H97" s="1" t="s">
+      <c r="H97" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="I97" s="2" t="s">
+      <c r="I97" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="1" t="n">
+      <c r="A98" s="2" t="n">
         <v>228620</v>
       </c>
-      <c r="B98" s="1" t="n">
+      <c r="B98" s="2" t="n">
         <v>231620</v>
       </c>
-      <c r="C98" s="1" t="s">
+      <c r="C98" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D98" s="1" t="s">
+      <c r="D98" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F98" s="1" t="s">
+      <c r="F98" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="I98" s="2" t="s">
+      <c r="I98" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="1" t="n">
+      <c r="A99" s="2" t="n">
         <v>231620</v>
       </c>
-      <c r="B99" s="1" t="n">
+      <c r="B99" s="2" t="n">
         <v>234620</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="C99" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D99" s="1" t="s">
+      <c r="D99" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="1" t="n">
+      <c r="A100" s="2" t="n">
         <v>234620</v>
       </c>
-      <c r="B100" s="1" t="n">
+      <c r="B100" s="2" t="n">
         <v>236620</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="C100" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D100" s="1" t="s">
+      <c r="D100" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="1" t="n">
+      <c r="A101" s="2" t="n">
         <v>236620</v>
       </c>
-      <c r="B101" s="1" t="n">
+      <c r="B101" s="2" t="n">
         <v>238620</v>
       </c>
-      <c r="C101" s="1" t="s">
+      <c r="C101" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D101" s="1" t="s">
+      <c r="D101" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="1" t="n">
+      <c r="A102" s="2" t="n">
         <v>238620</v>
       </c>
-      <c r="B102" s="1" t="n">
+      <c r="B102" s="2" t="n">
         <v>241620</v>
       </c>
-      <c r="C102" s="1" t="s">
+      <c r="C102" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D102" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E102" s="1" t="n">
+      <c r="D102" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E102" s="2" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="1" t="n">
+      <c r="A103" s="2" t="n">
         <v>241620</v>
       </c>
-      <c r="B103" s="1" t="n">
+      <c r="B103" s="2" t="n">
         <v>243620</v>
       </c>
-      <c r="C103" s="1" t="s">
+      <c r="C103" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D103" s="1" t="s">
+      <c r="D103" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="1" t="n">
+      <c r="A104" s="2" t="n">
         <v>241620</v>
       </c>
-      <c r="B104" s="1" t="n">
+      <c r="B104" s="2" t="n">
         <v>243620</v>
       </c>
-      <c r="C104" s="1" t="s">
+      <c r="C104" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D104" s="1" t="s">
+      <c r="D104" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F104" s="1" t="s">
+      <c r="F104" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I104" s="2" t="s">
+      <c r="I104" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="1" t="n">
+      <c r="A105" s="2" t="n">
         <v>243620</v>
       </c>
-      <c r="B105" s="1" t="n">
+      <c r="B105" s="2" t="n">
         <v>246620</v>
       </c>
-      <c r="C105" s="1" t="s">
+      <c r="C105" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D105" s="1" t="s">
+      <c r="D105" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="1" t="n">
+      <c r="A106" s="2" t="n">
         <v>246620</v>
       </c>
-      <c r="B106" s="1" t="n">
+      <c r="B106" s="2" t="n">
         <v>253260</v>
       </c>
-      <c r="C106" s="1" t="s">
+      <c r="C106" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D106" s="1" t="s">
+      <c r="D106" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F106" s="1" t="s">
+      <c r="F106" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I106" s="2" t="s">
+      <c r="I106" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="1" t="n">
+      <c r="A107" s="2" t="n">
         <v>246620</v>
       </c>
-      <c r="B107" s="1" t="n">
+      <c r="B107" s="2" t="n">
         <v>253260</v>
       </c>
-      <c r="C107" s="1" t="s">
+      <c r="C107" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D107" s="1" t="s">
+      <c r="D107" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="1" t="n">
+      <c r="A108" s="2" t="n">
         <v>253260</v>
       </c>
-      <c r="B108" s="1" t="n">
+      <c r="B108" s="2" t="n">
         <v>265020</v>
       </c>
-      <c r="C108" s="1" t="s">
+      <c r="C108" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="D108" s="1" t="s">
+      <c r="D108" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F108" s="1" t="s">
+      <c r="F108" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="H108" s="1" t="s">
+      <c r="H108" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="I108" s="2" t="s">
+      <c r="I108" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="1" t="n">
+      <c r="A109" s="2" t="n">
         <v>265020</v>
       </c>
-      <c r="B109" s="1" t="n">
+      <c r="B109" s="2" t="n">
         <v>271980</v>
       </c>
-      <c r="C109" s="3" t="s">
+      <c r="C109" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="D109" s="1" t="s">
+      <c r="D109" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="1" t="n">
+      <c r="A110" s="2" t="n">
         <v>265020</v>
       </c>
-      <c r="B110" s="1" t="n">
+      <c r="B110" s="2" t="n">
         <v>271980</v>
       </c>
-      <c r="C110" s="1" t="s">
+      <c r="C110" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D110" s="1" t="s">
+      <c r="D110" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E110" s="1" t="n">
+      <c r="E110" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="F110" s="1" t="s">
+      <c r="F110" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="H110" s="1" t="s">
+      <c r="H110" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="I110" s="2" t="s">
+      <c r="I110" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="1" t="n">
+      <c r="A111" s="2" t="n">
         <v>271980</v>
       </c>
-      <c r="B111" s="1" t="n">
+      <c r="B111" s="2" t="n">
         <v>273900</v>
       </c>
-      <c r="C111" s="3" t="s">
+      <c r="C111" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="D111" s="1" t="s">
+      <c r="D111" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="1" t="n">
+      <c r="A112" s="2" t="n">
         <v>273900</v>
       </c>
-      <c r="B112" s="1" t="n">
+      <c r="B112" s="2" t="n">
         <v>275020</v>
       </c>
-      <c r="C112" s="1" t="s">
+      <c r="C112" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="D112" s="1" t="s">
+      <c r="D112" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="1" t="n">
+      <c r="A113" s="2" t="n">
         <v>275020</v>
       </c>
-      <c r="B113" s="1" t="n">
+      <c r="B113" s="2" t="n">
         <v>279260</v>
       </c>
-      <c r="C113" s="1" t="s">
+      <c r="C113" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="D113" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E113" s="1" t="n">
+      <c r="D113" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E113" s="2" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="1" t="n">
+      <c r="A114" s="2" t="n">
         <v>279260</v>
       </c>
-      <c r="B114" s="1" t="n">
+      <c r="B114" s="2" t="n">
         <v>280260</v>
       </c>
-      <c r="C114" s="1" t="s">
+      <c r="C114" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D114" s="1" t="s">
+      <c r="D114" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F114" s="1" t="s">
+      <c r="F114" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="H114" s="1" t="s">
+      <c r="H114" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="I114" s="2" t="s">
+      <c r="I114" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="1" t="n">
+      <c r="A115" s="2" t="n">
         <v>280260</v>
       </c>
-      <c r="B115" s="1" t="n">
+      <c r="B115" s="2" t="n">
         <v>282260</v>
       </c>
-      <c r="C115" s="1" t="s">
+      <c r="C115" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D115" s="1" t="s">
+      <c r="D115" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="1" t="n">
+      <c r="A116" s="2" t="n">
         <v>282260</v>
       </c>
-      <c r="B116" s="1" t="n">
+      <c r="B116" s="2" t="n">
         <v>284260</v>
       </c>
-      <c r="C116" s="1" t="s">
+      <c r="C116" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="D116" s="1" t="s">
+      <c r="D116" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="1" t="n">
+      <c r="A117" s="2" t="n">
         <v>284260</v>
       </c>
-      <c r="B117" s="1" t="n">
+      <c r="B117" s="2" t="n">
         <v>287260</v>
       </c>
-      <c r="C117" s="1" t="s">
+      <c r="C117" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D117" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E117" s="1" t="n">
+      <c r="D117" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E117" s="2" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="1" t="n">
+      <c r="A118" s="2" t="n">
         <v>287260</v>
       </c>
-      <c r="B118" s="1" t="n">
+      <c r="B118" s="2" t="n">
         <v>288260</v>
       </c>
-      <c r="C118" s="1" t="s">
+      <c r="C118" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D118" s="1" t="s">
+      <c r="D118" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="1" t="n">
+      <c r="A119" s="2" t="n">
         <v>288260</v>
       </c>
-      <c r="B119" s="1" t="n">
+      <c r="B119" s="2" t="n">
         <v>292260</v>
       </c>
-      <c r="C119" s="1" t="s">
+      <c r="C119" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D119" s="1" t="s">
+      <c r="D119" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F119" s="1" t="s">
+      <c r="F119" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="H119" s="1" t="s">
+      <c r="H119" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="I119" s="2" t="s">
+      <c r="I119" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="1" t="n">
+      <c r="A120" s="2" t="n">
         <v>292260</v>
       </c>
-      <c r="B120" s="1" t="n">
+      <c r="B120" s="2" t="n">
         <v>294260</v>
       </c>
-      <c r="C120" s="1" t="s">
+      <c r="C120" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D120" s="1" t="s">
+      <c r="D120" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="1" t="n">
+      <c r="A121" s="2" t="n">
         <v>294260</v>
       </c>
-      <c r="B121" s="1" t="n">
+      <c r="B121" s="2" t="n">
         <v>299260</v>
       </c>
-      <c r="C121" s="1" t="s">
+      <c r="C121" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D121" s="1" t="s">
+      <c r="D121" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E121" s="1" t="n">
+      <c r="E121" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="F121" s="1" t="s">
+      <c r="F121" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="H121" s="1" t="s">
+      <c r="H121" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="I121" s="2" t="s">
+      <c r="I121" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="1" t="n">
+      <c r="A122" s="2" t="n">
         <v>299260</v>
       </c>
-      <c r="B122" s="1" t="n">
+      <c r="B122" s="2" t="n">
         <v>301260</v>
       </c>
-      <c r="C122" s="1" t="s">
+      <c r="C122" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="D122" s="1" t="s">
+      <c r="D122" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="1" t="n">
+      <c r="A123" s="2" t="n">
         <v>301260</v>
       </c>
-      <c r="B123" s="1" t="n">
+      <c r="B123" s="2" t="n">
         <v>302260</v>
       </c>
-      <c r="C123" s="1" t="s">
+      <c r="C123" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D123" s="1" t="s">
+      <c r="D123" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F123" s="1" t="s">
+      <c r="F123" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="H123" s="1" t="s">
+      <c r="H123" s="2"/>
+      <c r="I123" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="2" t="n">
+        <v>302260</v>
+      </c>
+      <c r="B124" s="2" t="n">
+        <v>304260</v>
+      </c>
+      <c r="C124" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="I123" s="2" t="s">
+      <c r="D124" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="2" t="n">
+        <v>304260</v>
+      </c>
+      <c r="B125" s="2" t="n">
+        <v>307260</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E125" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="2" t="n">
+        <v>307260</v>
+      </c>
+      <c r="B126" s="2" t="n">
+        <v>308260</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F126" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H126" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="I126" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="1" t="n">
-        <v>302260</v>
-      </c>
-      <c r="B124" s="1" t="n">
-        <v>304260</v>
-      </c>
-      <c r="C124" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D124" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="1" t="n">
-        <v>304260</v>
-      </c>
-      <c r="B125" s="1" t="n">
-        <v>307260</v>
-      </c>
-      <c r="C125" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D125" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E125" s="1" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="1" t="n">
-        <v>307260</v>
-      </c>
-      <c r="B126" s="1" t="n">
-        <v>308260</v>
-      </c>
-      <c r="C126" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D126" s="1" t="s">
+    <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="2" t="n">
+        <v>309260</v>
+      </c>
+      <c r="B127" s="2" t="n">
+        <v>320260</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D127" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E127" s="2" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="2" t="n">
+        <v>320260</v>
+      </c>
+      <c r="B128" s="2" t="n">
+        <v>321260</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D128" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F128" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I128" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="2" t="n">
+        <v>321260</v>
+      </c>
+      <c r="B129" s="2" t="n">
+        <v>323260</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D129" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="2" t="n">
+        <v>323260</v>
+      </c>
+      <c r="B130" s="2" t="n">
+        <v>326260</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D130" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F126" s="1" t="s">
+      <c r="F130" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="I130" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="2" t="n">
+        <v>326260</v>
+      </c>
+      <c r="B131" s="2" t="n">
+        <v>331260</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D131" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F131" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="H126" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="I126" s="2" t="s">
+      <c r="H131" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="I131" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="1" t="n">
-        <v>309260</v>
-      </c>
-      <c r="B127" s="1" t="n">
-        <v>320260</v>
-      </c>
-      <c r="C127" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D127" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E127" s="1" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="1" t="n">
-        <v>320260</v>
-      </c>
-      <c r="B128" s="1" t="n">
-        <v>321260</v>
-      </c>
-      <c r="C128" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D128" s="1" t="s">
+    <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="2" t="n">
+        <v>331260</v>
+      </c>
+      <c r="B132" s="2" t="n">
+        <v>335260</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D132" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="2" t="n">
+        <v>335260</v>
+      </c>
+      <c r="B133" s="2" t="n">
+        <v>339260</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D133" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E133" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="F133" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H133" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I133" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="2" t="n">
+        <v>339260</v>
+      </c>
+      <c r="B134" s="2" t="n">
+        <v>343260</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D134" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="2" t="n">
+        <v>343260</v>
+      </c>
+      <c r="B135" s="2" t="n">
+        <v>345260</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D135" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F128" s="1" t="s">
+      <c r="F135" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="2" t="n">
+        <v>345260</v>
+      </c>
+      <c r="B136" s="2" t="n">
+        <v>348260</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D136" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="2" t="n">
+        <v>348260</v>
+      </c>
+      <c r="B137" s="2" t="n">
+        <v>350260</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D137" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E137" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="F137" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I128" s="2" t="s">
+      <c r="H137" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="I137" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="1" t="n">
-        <v>321260</v>
-      </c>
-      <c r="B129" s="1" t="n">
-        <v>323260</v>
-      </c>
-      <c r="C129" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D129" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="1" t="n">
-        <v>323260</v>
-      </c>
-      <c r="B130" s="1" t="n">
-        <v>326260</v>
-      </c>
-      <c r="C130" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D130" s="1" t="s">
+    <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="2" t="n">
+        <v>350260</v>
+      </c>
+      <c r="B138" s="2" t="n">
+        <v>353260</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D138" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="2" t="n">
+        <v>353260</v>
+      </c>
+      <c r="B139" s="2" t="n">
+        <v>357260</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D139" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="2" t="n">
+        <v>357260</v>
+      </c>
+      <c r="B140" s="2" t="n">
+        <v>360260</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D140" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F130" s="1" t="s">
+      <c r="E140" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="F140" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H140" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="I140" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="2" t="n">
+        <v>360260</v>
+      </c>
+      <c r="B141" s="2" t="n">
+        <v>367260</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D141" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="2" t="n">
+        <v>367260</v>
+      </c>
+      <c r="B142" s="2" t="n">
+        <v>371260</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D142" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E142" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="F142" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H142" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="I142" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="2" t="n">
+        <v>371260</v>
+      </c>
+      <c r="B143" s="2" t="n">
+        <v>373260</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D143" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="2" t="n">
+        <v>373260</v>
+      </c>
+      <c r="B144" s="2" t="n">
+        <v>379260</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D144" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E144" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="F144" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H144" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="I144" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="2" t="n">
+        <v>383260</v>
+      </c>
+      <c r="B145" s="2" t="n">
+        <v>387260</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D145" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="2" t="n">
+        <v>387260</v>
+      </c>
+      <c r="B146" s="2" t="n">
+        <v>389260</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D146" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E146" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="F146" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H146" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I146" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="2" t="n">
+        <v>389260</v>
+      </c>
+      <c r="B147" s="2" t="n">
+        <v>394260</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D147" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="2" t="n">
+        <v>394260</v>
+      </c>
+      <c r="B148" s="2" t="n">
+        <v>396260</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D148" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E148" s="2" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="2" t="n">
+        <v>396260</v>
+      </c>
+      <c r="B149" s="2" t="n">
+        <v>398260</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D149" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F149" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H149" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I149" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="2" t="n">
+        <v>398260</v>
+      </c>
+      <c r="B150" s="2" t="n">
+        <v>401260</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D150" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F150" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="I130" s="2" t="s">
+    </row>
+    <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="2" t="n">
+        <v>401260</v>
+      </c>
+      <c r="B151" s="2" t="n">
+        <v>402260</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D151" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="2" t="n">
+        <v>402260</v>
+      </c>
+      <c r="B152" s="2" t="n">
+        <v>403260</v>
+      </c>
+      <c r="C152" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D152" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="2" t="n">
+        <v>403260</v>
+      </c>
+      <c r="B153" s="2" t="n">
+        <v>404260</v>
+      </c>
+      <c r="C153" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D153" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="2" t="n">
+        <v>404260</v>
+      </c>
+      <c r="B154" s="2" t="n">
+        <v>405260</v>
+      </c>
+      <c r="C154" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D154" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F154" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="2" t="n">
+        <v>405260</v>
+      </c>
+      <c r="B155" s="2" t="n">
+        <v>406260</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D155" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F155" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="2" t="n">
+        <v>406260</v>
+      </c>
+      <c r="B156" s="2" t="n">
+        <v>408260</v>
+      </c>
+      <c r="C156" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D156" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E156" s="2" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="2" t="n">
+        <v>408260</v>
+      </c>
+      <c r="B157" s="2" t="n">
+        <v>410260</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D157" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="2" t="n">
+        <v>410260</v>
+      </c>
+      <c r="B158" s="2" t="n">
+        <v>414260</v>
+      </c>
+      <c r="C158" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D158" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F158" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H158" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="I158" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="1" t="n">
-        <v>326260</v>
-      </c>
-      <c r="B131" s="1" t="n">
-        <v>331260</v>
-      </c>
-      <c r="C131" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D131" s="1" t="s">
+    <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="2" t="n">
+        <v>414260</v>
+      </c>
+      <c r="B159" s="2" t="n">
+        <v>416260</v>
+      </c>
+      <c r="C159" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D159" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="2" t="n">
+        <v>416260</v>
+      </c>
+      <c r="B160" s="2" t="n">
+        <v>418260</v>
+      </c>
+      <c r="C160" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D160" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F160" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="2" t="n">
+        <v>418260</v>
+      </c>
+      <c r="B161" s="2" t="n">
+        <v>419260</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D161" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F161" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="2" t="n">
+        <v>419260</v>
+      </c>
+      <c r="B162" s="2" t="n">
+        <v>420260</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D162" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="2" t="n">
+        <v>420260</v>
+      </c>
+      <c r="B163" s="2" t="n">
+        <v>423260</v>
+      </c>
+      <c r="C163" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D163" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="2" t="n">
+        <v>423260</v>
+      </c>
+      <c r="B164" s="2" t="n">
+        <v>424260</v>
+      </c>
+      <c r="C164" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D164" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="2" t="n">
+        <v>424260</v>
+      </c>
+      <c r="B165" s="2" t="n">
+        <v>425260</v>
+      </c>
+      <c r="C165" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D165" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F131" s="1" t="s">
+      <c r="F165" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="H131" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="I131" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="1" t="n">
-        <v>331260</v>
-      </c>
-      <c r="B132" s="1" t="n">
-        <v>335260</v>
-      </c>
-      <c r="C132" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D132" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="1" t="n">
-        <v>335260</v>
-      </c>
-      <c r="B133" s="1" t="n">
-        <v>339260</v>
-      </c>
-      <c r="C133" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D133" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E133" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="F133" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H133" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I133" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="1" t="n">
-        <v>339260</v>
-      </c>
-      <c r="B134" s="1" t="n">
-        <v>343260</v>
-      </c>
-      <c r="C134" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D134" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="1" t="n">
-        <v>343260</v>
-      </c>
-      <c r="B135" s="1" t="n">
-        <v>345260</v>
-      </c>
-      <c r="C135" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D135" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F135" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="1" t="n">
-        <v>345260</v>
-      </c>
-      <c r="B136" s="1" t="n">
-        <v>348260</v>
-      </c>
-      <c r="C136" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D136" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="1" t="n">
-        <v>348260</v>
-      </c>
-      <c r="B137" s="1" t="n">
-        <v>350260</v>
-      </c>
-      <c r="C137" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D137" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E137" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="F137" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H137" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="I137" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="1" t="n">
-        <v>350260</v>
-      </c>
-      <c r="B138" s="1" t="n">
-        <v>353260</v>
-      </c>
-      <c r="C138" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D138" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="1" t="n">
-        <v>353260</v>
-      </c>
-      <c r="B139" s="1" t="n">
-        <v>357260</v>
-      </c>
-      <c r="C139" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D139" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="1" t="n">
-        <v>357260</v>
-      </c>
-      <c r="B140" s="1" t="n">
-        <v>360260</v>
-      </c>
-      <c r="C140" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D140" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E140" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="F140" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H140" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="I140" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="1" t="n">
-        <v>360260</v>
-      </c>
-      <c r="B141" s="1" t="n">
-        <v>367260</v>
-      </c>
-      <c r="C141" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D141" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="1" t="n">
-        <v>367260</v>
-      </c>
-      <c r="B142" s="1" t="n">
-        <v>371260</v>
-      </c>
-      <c r="C142" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D142" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E142" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="F142" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H142" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="I142" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="1" t="n">
-        <v>371260</v>
-      </c>
-      <c r="B143" s="1" t="n">
-        <v>373260</v>
-      </c>
-      <c r="C143" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D143" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="1" t="n">
-        <v>373260</v>
-      </c>
-      <c r="B144" s="1" t="n">
-        <v>379260</v>
-      </c>
-      <c r="C144" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D144" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E144" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="F144" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H144" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="I144" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="1" t="n">
-        <v>383260</v>
-      </c>
-      <c r="B145" s="1" t="n">
-        <v>387260</v>
-      </c>
-      <c r="C145" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="D145" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="1" t="n">
-        <v>387260</v>
-      </c>
-      <c r="B146" s="1" t="n">
-        <v>389260</v>
-      </c>
-      <c r="C146" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D146" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E146" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="F146" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H146" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="I146" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="1" t="n">
-        <v>389260</v>
-      </c>
-      <c r="B147" s="1" t="n">
-        <v>394260</v>
-      </c>
-      <c r="C147" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="D147" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="1" t="n">
-        <v>394260</v>
-      </c>
-      <c r="B148" s="1" t="n">
-        <v>396260</v>
-      </c>
-      <c r="C148" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D148" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E148" s="1" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="1" t="n">
-        <v>396260</v>
-      </c>
-      <c r="B149" s="1" t="n">
-        <v>398260</v>
-      </c>
-      <c r="C149" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D149" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F149" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H149" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I149" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="1" t="n">
-        <v>398260</v>
-      </c>
-      <c r="B150" s="1" t="n">
-        <v>401260</v>
-      </c>
-      <c r="C150" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D150" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F150" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="1" t="n">
-        <v>401260</v>
-      </c>
-      <c r="B151" s="1" t="n">
-        <v>402260</v>
-      </c>
-      <c r="C151" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="D151" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="1" t="n">
-        <v>402260</v>
-      </c>
-      <c r="B152" s="1" t="n">
-        <v>403260</v>
-      </c>
-      <c r="C152" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D152" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="1" t="n">
-        <v>403260</v>
-      </c>
-      <c r="B153" s="1" t="n">
-        <v>404260</v>
-      </c>
-      <c r="C153" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D153" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="1" t="n">
-        <v>404260</v>
-      </c>
-      <c r="B154" s="1" t="n">
-        <v>405260</v>
-      </c>
-      <c r="C154" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D154" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F154" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="1" t="n">
-        <v>405260</v>
-      </c>
-      <c r="B155" s="1" t="n">
-        <v>406260</v>
-      </c>
-      <c r="C155" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D155" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F155" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="1" t="n">
-        <v>406260</v>
-      </c>
-      <c r="B156" s="1" t="n">
-        <v>408260</v>
-      </c>
-      <c r="C156" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D156" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E156" s="1" t="n">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="1" t="n">
-        <v>408260</v>
-      </c>
-      <c r="B157" s="1" t="n">
-        <v>410260</v>
-      </c>
-      <c r="C157" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D157" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="1" t="n">
-        <v>410260</v>
-      </c>
-      <c r="B158" s="1" t="n">
-        <v>414260</v>
-      </c>
-      <c r="C158" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="D158" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F158" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H158" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I158" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="1" t="n">
-        <v>414260</v>
-      </c>
-      <c r="B159" s="1" t="n">
-        <v>416260</v>
-      </c>
-      <c r="C159" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D159" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="1" t="n">
-        <v>416260</v>
-      </c>
-      <c r="B160" s="1" t="n">
-        <v>418260</v>
-      </c>
-      <c r="C160" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D160" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F160" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="1" t="n">
-        <v>418260</v>
-      </c>
-      <c r="B161" s="1" t="n">
-        <v>419260</v>
-      </c>
-      <c r="C161" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D161" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F161" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="1" t="n">
-        <v>419260</v>
-      </c>
-      <c r="B162" s="1" t="n">
-        <v>420260</v>
-      </c>
-      <c r="C162" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D162" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="1" t="n">
-        <v>420260</v>
-      </c>
-      <c r="B163" s="1" t="n">
-        <v>423260</v>
-      </c>
-      <c r="C163" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="D163" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="1" t="n">
-        <v>423260</v>
-      </c>
-      <c r="B164" s="1" t="n">
-        <v>424260</v>
-      </c>
-      <c r="C164" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D164" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="1" t="n">
-        <v>424260</v>
-      </c>
-      <c r="B165" s="1" t="n">
+    </row>
+    <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="2" t="n">
         <v>425260</v>
       </c>
-      <c r="C165" s="1" t="s">
+      <c r="B166" s="2" t="n">
+        <v>426260</v>
+      </c>
+      <c r="C166" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="D165" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F165" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="1" t="n">
-        <v>425260</v>
-      </c>
-      <c r="B166" s="1" t="n">
+      <c r="D166" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="2" t="n">
         <v>426260</v>
       </c>
-      <c r="C166" s="1" t="s">
+      <c r="B167" s="2" t="n">
+        <v>428260</v>
+      </c>
+      <c r="C167" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="D166" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="1" t="n">
-        <v>426260</v>
-      </c>
-      <c r="B167" s="1" t="n">
+      <c r="D167" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="2" t="n">
         <v>428260</v>
       </c>
-      <c r="C167" s="1" t="s">
+      <c r="B168" s="2" t="n">
+        <v>430260</v>
+      </c>
+      <c r="C168" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="D167" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="1" t="n">
-        <v>428260</v>
-      </c>
-      <c r="B168" s="1" t="n">
-        <v>430260</v>
-      </c>
-      <c r="C168" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D168" s="1" t="s">
+      <c r="D168" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>